<commit_message>
added info and tableau synthèse
</commit_message>
<xml_diff>
--- a/assets/tableau_synthese.xlsx
+++ b/assets/tableau_synthese.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laetitia\Documents\Cours\BTS_SIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucaa\Desktop\ipssi\portfolio\real\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F768446A-5B90-43C7-A9D5-F77B01FC03F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2049A7BD-8C62-462E-85B9-155908D42370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="45945" yWindow="7290" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -96,13 +96,7 @@
 ▸Développer son projet professionnel</t>
   </si>
   <si>
-    <t>Centre de formation :</t>
-  </si>
-  <si>
     <t>▢ SISR</t>
-  </si>
-  <si>
-    <t>▢ SLAM</t>
   </si>
   <si>
     <t xml:space="preserve">Réalisation en cours de formation
@@ -120,9 +114,6 @@
     <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
-    <t xml:space="preserve">NOM et prénom : </t>
-  </si>
-  <si>
     <t>Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
   </si>
   <si>
@@ -133,6 +124,51 @@
   </si>
   <si>
     <t>Adresse URL du portfolio :</t>
+  </si>
+  <si>
+    <t>X SLAM</t>
+  </si>
+  <si>
+    <t>NOM et prénom : Luca Améaume</t>
+  </si>
+  <si>
+    <t>Centre de formation : IPSSI FORMATION</t>
+  </si>
+  <si>
+    <t>AP1: Création d'une entreprise et de son site web.</t>
+  </si>
+  <si>
+    <t>15/09/2021 au 03/12/2021</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>13/05/2022 au 20/06/2022</t>
+  </si>
+  <si>
+    <t>AP3: Création d'un application légèrde avec une API pour l'entreprise M2L</t>
+  </si>
+  <si>
+    <t>AP2:  Proposer des solutions aux problèmatiques de l'entreprise m2l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/10/2022 au XX </t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t>01/01/2017 au XX</t>
+  </si>
+  <si>
+    <t>Linkdn</t>
+  </si>
+  <si>
+    <t>XXXX au XXXX</t>
   </si>
 </sst>
 </file>
@@ -142,7 +178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -204,6 +240,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -604,7 +655,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -675,9 +726,54 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -702,50 +798,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -766,7 +838,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1091,98 +1163,98 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="8" width="30.7109375" style="1" customWidth="1"/>
-    <col min="9" max="43" width="11.42578125" customWidth="1"/>
-    <col min="44" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="70.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="30.7265625" style="1" customWidth="1"/>
+    <col min="9" max="43" width="11.453125" customWidth="1"/>
+    <col min="44" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="24"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="32"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3" s="47"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+    <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="45"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>23</v>
+      <c r="B6" s="35" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>0</v>
@@ -1203,30 +1275,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="46" t="s">
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="46" t="s">
+      <c r="G7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="47" t="s">
+      <c r="H7" s="25" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
-      <c r="K7"/>
+      <c r="K7" s="49"/>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>
@@ -1260,17 +1332,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1307,12 +1379,18 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="8"/>
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>28</v>
+      </c>
       <c r="C9" s="16"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="E9" s="51" t="s">
+        <v>29</v>
+      </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
@@ -1352,14 +1430,20 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="8"/>
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>31</v>
+      </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="F10" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="52"/>
       <c r="H10" s="18"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -1397,14 +1481,24 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="8"/>
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>34</v>
+      </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="E11" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="52" t="s">
+        <v>30</v>
+      </c>
       <c r="H11" s="18"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -1442,15 +1536,21 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="8"/>
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>36</v>
+      </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
+      <c r="H12" s="54" t="s">
+        <v>30</v>
+      </c>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1487,15 +1587,21 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="8"/>
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
+      <c r="H13" s="54" t="s">
+        <v>29</v>
+      </c>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1532,7 +1638,7 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="8"/>
       <c r="C14" s="17"/>
@@ -1577,7 +1683,7 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="8"/>
       <c r="C15" s="17"/>
@@ -1622,7 +1728,7 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="8"/>
       <c r="C16" s="17"/>
@@ -1667,7 +1773,7 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="8"/>
       <c r="C17" s="17"/>
@@ -1712,7 +1818,7 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="8"/>
       <c r="C18" s="17"/>
@@ -1757,17 +1863,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1804,7 +1910,7 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="8"/>
       <c r="C20" s="17"/>
@@ -1849,7 +1955,7 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="8"/>
       <c r="C21" s="17"/>
@@ -1894,7 +2000,7 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="8"/>
       <c r="C22" s="17"/>
@@ -1939,7 +2045,7 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="8"/>
       <c r="C23" s="17"/>
@@ -1984,7 +2090,7 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="8"/>
       <c r="C24" s="17"/>
@@ -2029,7 +2135,7 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="8"/>
       <c r="C25" s="17"/>
@@ -2074,7 +2180,7 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="8"/>
       <c r="C26" s="17"/>
@@ -2119,17 +2225,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2166,7 +2272,7 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="8"/>
       <c r="C28" s="17"/>
@@ -2211,7 +2317,7 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="8"/>
       <c r="C29" s="17"/>
@@ -2256,7 +2362,7 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="8"/>
       <c r="C30" s="17"/>
@@ -2301,7 +2407,7 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="8"/>
       <c r="C31" s="17"/>
@@ -2346,7 +2452,7 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="8"/>
       <c r="C32" s="17"/>
@@ -2391,7 +2497,7 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="9"/>
       <c r="C33" s="19"/>
@@ -2436,7 +2542,7 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
       <c r="B34" s="13"/>
       <c r="C34" s="21"/>
@@ -2481,7 +2587,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2526,54 +2632,59 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2581,16 +2692,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="48" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed responsive on pdf
</commit_message>
<xml_diff>
--- a/assets/tableau_synthese.xlsx
+++ b/assets/tableau_synthese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucaA\Desktop\ipssi\portfolio\real\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384578B8-BFF1-45B6-BCDC-1A542B4F2C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA9470D-3CD6-4B5A-931F-7DB70B3E983D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$34</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -141,9 +141,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>13/05/2022 au 20/06/2022</t>
   </si>
   <si>
@@ -172,6 +169,27 @@
   </si>
   <si>
     <t xml:space="preserve">Gestion du support et bug reports joueurs via un système de ticket et de validation manuel. </t>
+  </si>
+  <si>
+    <t>Installation et modifications d'un thème d'un CMS et de service de payement</t>
+  </si>
+  <si>
+    <t>24/10/2022 au 25/10/2022</t>
+  </si>
+  <si>
+    <t>27/10/2022 au 28/10/2022</t>
+  </si>
+  <si>
+    <t>Analyse de problème d'optimisation via un outil de profiler (spark et yourkit)</t>
+  </si>
+  <si>
+    <t>05/04/2022 au 07/04/2022</t>
+  </si>
+  <si>
+    <t>Mise en place d'un service de tâche (Notion)</t>
+  </si>
+  <si>
+    <t>07/11/2022 au 07/11/2022</t>
   </si>
 </sst>
 </file>
@@ -181,7 +199,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -244,17 +262,7 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="24"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="28"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -658,7 +666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -735,14 +743,35 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -750,9 +779,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -784,30 +810,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1152,10 +1154,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ81"/>
+  <dimension ref="A1:AQ80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1168,56 +1170,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="31"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="49" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="50"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="35"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
@@ -1229,22 +1231,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="42"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="44" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1267,8 +1269,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="20" t="s">
         <v>9</v>
       </c>
@@ -1324,16 +1326,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="40"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1372,7 +1374,7 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>27</v>
@@ -1423,18 +1425,18 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="26"/>
+      <c r="F10" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="25"/>
       <c r="H10" s="16"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -1473,14 +1475,20 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="16"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="26" t="s">
+        <v>28</v>
+      </c>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1519,18 +1527,18 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
-      <c r="H12" s="28" t="s">
-        <v>29</v>
+      <c r="H12" s="26" t="s">
+        <v>28</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1569,20 +1577,14 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>36</v>
-      </c>
+      <c r="A13" s="9"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="28" t="s">
-        <v>28</v>
-      </c>
+      <c r="H13" s="16"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1799,15 +1801,17 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="43"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1844,17 +1848,21 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="16"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1893,12 +1901,12 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="25" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="15"/>
@@ -2167,15 +2175,17 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16"/>
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2212,17 +2222,21 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="16"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2263,14 +2277,16 @@
       <c r="A28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="22" t="s">
+        <v>41</v>
+      </c>
       <c r="C28" s="15"/>
-      <c r="D28" s="26" t="s">
-        <v>28</v>
-      </c>
+      <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
+      <c r="G28" s="25" t="s">
+        <v>28</v>
+      </c>
       <c r="H28" s="16"/>
       <c r="I28"/>
       <c r="J28"/>
@@ -2309,12 +2325,18 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
+      <c r="F29" s="25" t="s">
+        <v>28</v>
+      </c>
       <c r="G29" s="15"/>
       <c r="H29" s="16"/>
       <c r="I29"/>
@@ -2488,15 +2510,15 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="16"/>
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="18"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2533,15 +2555,15 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="18"/>
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2578,51 +2600,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-      <c r="AF35"/>
-      <c r="AG35"/>
-      <c r="AH35"/>
-      <c r="AI35"/>
-      <c r="AJ35"/>
-      <c r="AK35"/>
-      <c r="AL35"/>
-      <c r="AM35"/>
-      <c r="AN35"/>
-      <c r="AO35"/>
-      <c r="AP35"/>
-      <c r="AQ35"/>
-    </row>
+    <row r="35" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2668,21 +2646,20 @@
     <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A5:H5"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>